<commit_message>
error corrections - based on issues found in storyline production - and re-calculate reporting data
</commit_message>
<xml_diff>
--- a/Output/2023/116-17.18.2-1827-SG_STT_FPOS-1132.xlsx
+++ b/Output/2023/116-17.18.2-1827-SG_STT_FPOS-1132.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="612">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="618">
   <si>
     <t xml:space="preserve">Indicator</t>
   </si>
@@ -1851,6 +1851,24 @@
   </si>
   <si>
     <t xml:space="preserve">Regional</t>
+  </si>
+  <si>
+    <t xml:space="preserve">147</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">141</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25</t>
   </si>
 </sst>
 </file>
@@ -2252,7 +2270,7 @@
         <v>2022</v>
       </c>
       <c r="G2" t="s">
-        <v>33</v>
+        <v>612</v>
       </c>
       <c r="H2" t="n">
         <v>2022</v>
@@ -2302,7 +2320,7 @@
         <v>2022</v>
       </c>
       <c r="G3" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="H3" t="n">
         <v>2022</v>
@@ -2352,7 +2370,7 @@
         <v>2022</v>
       </c>
       <c r="G4" t="s">
-        <v>33</v>
+        <v>149</v>
       </c>
       <c r="H4" t="n">
         <v>2022</v>
@@ -2402,7 +2420,7 @@
         <v>2022</v>
       </c>
       <c r="G5" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="H5" t="n">
         <v>2022</v>
@@ -2452,7 +2470,7 @@
         <v>2022</v>
       </c>
       <c r="G6" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="H6" t="n">
         <v>2022</v>
@@ -2502,7 +2520,7 @@
         <v>2022</v>
       </c>
       <c r="G7" t="s">
-        <v>33</v>
+        <v>149</v>
       </c>
       <c r="H7" t="n">
         <v>2022</v>
@@ -2552,7 +2570,7 @@
         <v>2022</v>
       </c>
       <c r="G8" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="H8" t="n">
         <v>2022</v>
@@ -2602,7 +2620,7 @@
         <v>2022</v>
       </c>
       <c r="G9" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="H9" t="n">
         <v>2022</v>
@@ -2652,7 +2670,7 @@
         <v>2022</v>
       </c>
       <c r="G10" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="H10" t="n">
         <v>2022</v>
@@ -2702,7 +2720,7 @@
         <v>2022</v>
       </c>
       <c r="G11" t="s">
-        <v>33</v>
+        <v>62</v>
       </c>
       <c r="H11" t="n">
         <v>2022</v>
@@ -2752,7 +2770,7 @@
         <v>2022</v>
       </c>
       <c r="G12" t="s">
-        <v>33</v>
+        <v>68</v>
       </c>
       <c r="H12" t="n">
         <v>2022</v>
@@ -2802,7 +2820,7 @@
         <v>2022</v>
       </c>
       <c r="G13" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="H13" t="n">
         <v>2022</v>
@@ -2852,7 +2870,7 @@
         <v>2022</v>
       </c>
       <c r="G14" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="H14" t="n">
         <v>2022</v>
@@ -2902,7 +2920,7 @@
         <v>2022</v>
       </c>
       <c r="G15" t="s">
-        <v>33</v>
+        <v>52</v>
       </c>
       <c r="H15" t="n">
         <v>2022</v>
@@ -2952,7 +2970,7 @@
         <v>2022</v>
       </c>
       <c r="G16" t="s">
-        <v>33</v>
+        <v>80</v>
       </c>
       <c r="H16" t="n">
         <v>2022</v>
@@ -3002,7 +3020,7 @@
         <v>2022</v>
       </c>
       <c r="G17" t="s">
-        <v>33</v>
+        <v>62</v>
       </c>
       <c r="H17" t="n">
         <v>2022</v>
@@ -3052,7 +3070,7 @@
         <v>2022</v>
       </c>
       <c r="G18" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="H18" t="n">
         <v>2022</v>
@@ -3102,7 +3120,7 @@
         <v>2022</v>
       </c>
       <c r="G19" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="H19" t="n">
         <v>2022</v>
@@ -3152,7 +3170,7 @@
         <v>2022</v>
       </c>
       <c r="G20" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="H20" t="n">
         <v>2022</v>
@@ -3202,7 +3220,7 @@
         <v>2022</v>
       </c>
       <c r="G21" t="s">
-        <v>33</v>
+        <v>52</v>
       </c>
       <c r="H21" t="n">
         <v>2022</v>
@@ -3252,7 +3270,7 @@
         <v>2022</v>
       </c>
       <c r="G22" t="s">
-        <v>33</v>
+        <v>155</v>
       </c>
       <c r="H22" t="n">
         <v>2022</v>
@@ -3302,7 +3320,7 @@
         <v>2022</v>
       </c>
       <c r="G23" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="H23" t="n">
         <v>2022</v>
@@ -3352,7 +3370,7 @@
         <v>2022</v>
       </c>
       <c r="G24" t="s">
-        <v>33</v>
+        <v>149</v>
       </c>
       <c r="H24" t="n">
         <v>2022</v>
@@ -3402,7 +3420,7 @@
         <v>2022</v>
       </c>
       <c r="G25" t="s">
-        <v>33</v>
+        <v>154</v>
       </c>
       <c r="H25" t="n">
         <v>2022</v>
@@ -3452,7 +3470,7 @@
         <v>2022</v>
       </c>
       <c r="G26" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="H26" t="n">
         <v>2022</v>
@@ -3502,7 +3520,7 @@
         <v>2022</v>
       </c>
       <c r="G27" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="H27" t="n">
         <v>2022</v>
@@ -3552,7 +3570,7 @@
         <v>2022</v>
       </c>
       <c r="G28" t="s">
-        <v>33</v>
+        <v>68</v>
       </c>
       <c r="H28" t="n">
         <v>2022</v>
@@ -3602,7 +3620,7 @@
         <v>2022</v>
       </c>
       <c r="G29" t="s">
-        <v>33</v>
+        <v>613</v>
       </c>
       <c r="H29" t="n">
         <v>2022</v>
@@ -3652,7 +3670,7 @@
         <v>2022</v>
       </c>
       <c r="G30" t="s">
-        <v>33</v>
+        <v>614</v>
       </c>
       <c r="H30" t="n">
         <v>2022</v>
@@ -3702,7 +3720,7 @@
         <v>2022</v>
       </c>
       <c r="G31" t="s">
-        <v>33</v>
+        <v>507</v>
       </c>
       <c r="H31" t="n">
         <v>2022</v>
@@ -3752,7 +3770,7 @@
         <v>2022</v>
       </c>
       <c r="G32" t="s">
-        <v>33</v>
+        <v>615</v>
       </c>
       <c r="H32" t="n">
         <v>2022</v>
@@ -3802,7 +3820,7 @@
         <v>2022</v>
       </c>
       <c r="G33" t="s">
-        <v>33</v>
+        <v>380</v>
       </c>
       <c r="H33" t="n">
         <v>2022</v>
@@ -3852,7 +3870,7 @@
         <v>2022</v>
       </c>
       <c r="G34" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="H34" t="n">
         <v>2022</v>
@@ -3902,7 +3920,7 @@
         <v>2022</v>
       </c>
       <c r="G35" t="s">
-        <v>33</v>
+        <v>332</v>
       </c>
       <c r="H35" t="n">
         <v>2022</v>
@@ -3952,7 +3970,7 @@
         <v>2022</v>
       </c>
       <c r="G36" t="s">
-        <v>33</v>
+        <v>322</v>
       </c>
       <c r="H36" t="n">
         <v>2022</v>
@@ -4002,7 +4020,7 @@
         <v>2022</v>
       </c>
       <c r="G37" t="s">
-        <v>33</v>
+        <v>320</v>
       </c>
       <c r="H37" t="n">
         <v>2022</v>
@@ -8352,7 +8370,7 @@
         <v>2022</v>
       </c>
       <c r="G124" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="H124" t="n">
         <v>2022</v>
@@ -9352,7 +9370,7 @@
         <v>2022</v>
       </c>
       <c r="G144" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="H144" t="n">
         <v>2022</v>
@@ -10352,7 +10370,7 @@
         <v>2022</v>
       </c>
       <c r="G164" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="H164" t="n">
         <v>2022</v>
@@ -16402,7 +16420,7 @@
         <v>2021</v>
       </c>
       <c r="G285" t="s">
-        <v>33</v>
+        <v>616</v>
       </c>
       <c r="H285" t="n">
         <v>2021</v>
@@ -16452,7 +16470,7 @@
         <v>2021</v>
       </c>
       <c r="G286" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="H286" t="n">
         <v>2021</v>
@@ -16502,7 +16520,7 @@
         <v>2021</v>
       </c>
       <c r="G287" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="H287" t="n">
         <v>2021</v>
@@ -16552,7 +16570,7 @@
         <v>2021</v>
       </c>
       <c r="G288" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="H288" t="n">
         <v>2021</v>
@@ -16602,7 +16620,7 @@
         <v>2021</v>
       </c>
       <c r="G289" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="H289" t="n">
         <v>2021</v>
@@ -16652,7 +16670,7 @@
         <v>2021</v>
       </c>
       <c r="G290" t="s">
-        <v>33</v>
+        <v>149</v>
       </c>
       <c r="H290" t="n">
         <v>2021</v>
@@ -16702,7 +16720,7 @@
         <v>2021</v>
       </c>
       <c r="G291" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="H291" t="n">
         <v>2021</v>
@@ -16752,7 +16770,7 @@
         <v>2021</v>
       </c>
       <c r="G292" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="H292" t="n">
         <v>2021</v>
@@ -16802,7 +16820,7 @@
         <v>2021</v>
       </c>
       <c r="G293" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="H293" t="n">
         <v>2021</v>
@@ -16852,7 +16870,7 @@
         <v>2021</v>
       </c>
       <c r="G294" t="s">
-        <v>33</v>
+        <v>62</v>
       </c>
       <c r="H294" t="n">
         <v>2021</v>
@@ -16902,7 +16920,7 @@
         <v>2021</v>
       </c>
       <c r="G295" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="H295" t="n">
         <v>2021</v>
@@ -16952,7 +16970,7 @@
         <v>2021</v>
       </c>
       <c r="G296" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="H296" t="n">
         <v>2021</v>
@@ -17002,7 +17020,7 @@
         <v>2021</v>
       </c>
       <c r="G297" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="H297" t="n">
         <v>2021</v>
@@ -17052,7 +17070,7 @@
         <v>2021</v>
       </c>
       <c r="G298" t="s">
-        <v>33</v>
+        <v>76</v>
       </c>
       <c r="H298" t="n">
         <v>2021</v>
@@ -17102,7 +17120,7 @@
         <v>2021</v>
       </c>
       <c r="G299" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="H299" t="n">
         <v>2021</v>
@@ -17152,7 +17170,7 @@
         <v>2021</v>
       </c>
       <c r="G300" t="s">
-        <v>33</v>
+        <v>62</v>
       </c>
       <c r="H300" t="n">
         <v>2021</v>
@@ -17202,7 +17220,7 @@
         <v>2021</v>
       </c>
       <c r="G301" t="s">
-        <v>33</v>
+        <v>62</v>
       </c>
       <c r="H301" t="n">
         <v>2021</v>
@@ -17252,7 +17270,7 @@
         <v>2021</v>
       </c>
       <c r="G302" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="H302" t="n">
         <v>2021</v>
@@ -17302,7 +17320,7 @@
         <v>2021</v>
       </c>
       <c r="G303" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="H303" t="n">
         <v>2021</v>
@@ -17352,7 +17370,7 @@
         <v>2021</v>
       </c>
       <c r="G304" t="s">
-        <v>33</v>
+        <v>52</v>
       </c>
       <c r="H304" t="n">
         <v>2021</v>
@@ -17402,7 +17420,7 @@
         <v>2021</v>
       </c>
       <c r="G305" t="s">
-        <v>33</v>
+        <v>155</v>
       </c>
       <c r="H305" t="n">
         <v>2021</v>
@@ -17452,7 +17470,7 @@
         <v>2021</v>
       </c>
       <c r="G306" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="H306" t="n">
         <v>2021</v>
@@ -17502,7 +17520,7 @@
         <v>2021</v>
       </c>
       <c r="G307" t="s">
-        <v>33</v>
+        <v>150</v>
       </c>
       <c r="H307" t="n">
         <v>2021</v>
@@ -17552,7 +17570,7 @@
         <v>2021</v>
       </c>
       <c r="G308" t="s">
-        <v>33</v>
+        <v>155</v>
       </c>
       <c r="H308" t="n">
         <v>2021</v>
@@ -17602,7 +17620,7 @@
         <v>2021</v>
       </c>
       <c r="G309" t="s">
-        <v>33</v>
+        <v>76</v>
       </c>
       <c r="H309" t="n">
         <v>2021</v>
@@ -17652,7 +17670,7 @@
         <v>2021</v>
       </c>
       <c r="G310" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="H310" t="n">
         <v>2021</v>
@@ -17702,7 +17720,7 @@
         <v>2021</v>
       </c>
       <c r="G311" t="s">
-        <v>33</v>
+        <v>76</v>
       </c>
       <c r="H311" t="n">
         <v>2021</v>
@@ -17752,7 +17770,7 @@
         <v>2021</v>
       </c>
       <c r="G312" t="s">
-        <v>33</v>
+        <v>617</v>
       </c>
       <c r="H312" t="n">
         <v>2021</v>
@@ -17802,7 +17820,7 @@
         <v>2021</v>
       </c>
       <c r="G313" t="s">
-        <v>33</v>
+        <v>614</v>
       </c>
       <c r="H313" t="n">
         <v>2021</v>
@@ -17852,7 +17870,7 @@
         <v>2021</v>
       </c>
       <c r="G314" t="s">
-        <v>33</v>
+        <v>322</v>
       </c>
       <c r="H314" t="n">
         <v>2021</v>
@@ -17902,7 +17920,7 @@
         <v>2021</v>
       </c>
       <c r="G315" t="s">
-        <v>33</v>
+        <v>332</v>
       </c>
       <c r="H315" t="n">
         <v>2021</v>
@@ -17952,7 +17970,7 @@
         <v>2021</v>
       </c>
       <c r="G316" t="s">
-        <v>33</v>
+        <v>381</v>
       </c>
       <c r="H316" t="n">
         <v>2021</v>
@@ -18002,7 +18020,7 @@
         <v>2021</v>
       </c>
       <c r="G317" t="s">
-        <v>33</v>
+        <v>52</v>
       </c>
       <c r="H317" t="n">
         <v>2021</v>
@@ -18052,7 +18070,7 @@
         <v>2021</v>
       </c>
       <c r="G318" t="s">
-        <v>33</v>
+        <v>507</v>
       </c>
       <c r="H318" t="n">
         <v>2021</v>
@@ -18102,7 +18120,7 @@
         <v>2021</v>
       </c>
       <c r="G319" t="s">
-        <v>33</v>
+        <v>507</v>
       </c>
       <c r="H319" t="n">
         <v>2021</v>
@@ -18152,7 +18170,7 @@
         <v>2021</v>
       </c>
       <c r="G320" t="s">
-        <v>33</v>
+        <v>150</v>
       </c>
       <c r="H320" t="n">
         <v>2021</v>
@@ -18252,7 +18270,7 @@
         <v>2021</v>
       </c>
       <c r="G322" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="H322" t="n">
         <v>2021</v>
@@ -19202,7 +19220,7 @@
         <v>2021</v>
       </c>
       <c r="G341" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="H341" t="n">
         <v>2021</v>
@@ -19752,7 +19770,7 @@
         <v>2021</v>
       </c>
       <c r="G352" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="H352" t="n">
         <v>2021</v>
@@ -22502,7 +22520,7 @@
         <v>2021</v>
       </c>
       <c r="G407" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="H407" t="n">
         <v>2021</v>
@@ -23502,7 +23520,7 @@
         <v>2021</v>
       </c>
       <c r="G427" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="H427" t="n">
         <v>2021</v>
@@ -24502,7 +24520,7 @@
         <v>2021</v>
       </c>
       <c r="G447" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="H447" t="n">
         <v>2021</v>
@@ -24602,7 +24620,7 @@
         <v>2021</v>
       </c>
       <c r="G449" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="H449" t="n">
         <v>2021</v>
@@ -28652,7 +28670,7 @@
         <v>2021</v>
       </c>
       <c r="G530" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="H530" t="n">
         <v>2021</v>
@@ -30552,7 +30570,7 @@
         <v>2020</v>
       </c>
       <c r="G568" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="H568" t="n">
         <v>2020</v>
@@ -30602,7 +30620,7 @@
         <v>2020</v>
       </c>
       <c r="G569" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="H569" t="n">
         <v>2020</v>
@@ -30652,7 +30670,7 @@
         <v>2020</v>
       </c>
       <c r="G570" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="H570" t="n">
         <v>2020</v>
@@ -30702,7 +30720,7 @@
         <v>2020</v>
       </c>
       <c r="G571" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="H571" t="n">
         <v>2020</v>
@@ -30752,7 +30770,7 @@
         <v>2020</v>
       </c>
       <c r="G572" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="H572" t="n">
         <v>2020</v>
@@ -30802,7 +30820,7 @@
         <v>2020</v>
       </c>
       <c r="G573" t="s">
-        <v>33</v>
+        <v>52</v>
       </c>
       <c r="H573" t="n">
         <v>2020</v>
@@ -30852,7 +30870,7 @@
         <v>2020</v>
       </c>
       <c r="G574" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="H574" t="n">
         <v>2020</v>
@@ -30902,7 +30920,7 @@
         <v>2020</v>
       </c>
       <c r="G575" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="H575" t="n">
         <v>2020</v>
@@ -30952,7 +30970,7 @@
         <v>2020</v>
       </c>
       <c r="G576" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="H576" t="n">
         <v>2020</v>
@@ -31002,7 +31020,7 @@
         <v>2020</v>
       </c>
       <c r="G577" t="s">
-        <v>33</v>
+        <v>62</v>
       </c>
       <c r="H577" t="n">
         <v>2020</v>
@@ -31052,7 +31070,7 @@
         <v>2020</v>
       </c>
       <c r="G578" t="s">
-        <v>33</v>
+        <v>68</v>
       </c>
       <c r="H578" t="n">
         <v>2020</v>
@@ -31102,7 +31120,7 @@
         <v>2020</v>
       </c>
       <c r="G579" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="H579" t="n">
         <v>2020</v>
@@ -31152,7 +31170,7 @@
         <v>2020</v>
       </c>
       <c r="G580" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="H580" t="n">
         <v>2020</v>
@@ -31202,7 +31220,7 @@
         <v>2020</v>
       </c>
       <c r="G581" t="s">
-        <v>33</v>
+        <v>68</v>
       </c>
       <c r="H581" t="n">
         <v>2020</v>
@@ -31252,7 +31270,7 @@
         <v>2020</v>
       </c>
       <c r="G582" t="s">
-        <v>33</v>
+        <v>80</v>
       </c>
       <c r="H582" t="n">
         <v>2020</v>
@@ -31302,7 +31320,7 @@
         <v>2020</v>
       </c>
       <c r="G583" t="s">
-        <v>33</v>
+        <v>62</v>
       </c>
       <c r="H583" t="n">
         <v>2020</v>
@@ -31352,7 +31370,7 @@
         <v>2020</v>
       </c>
       <c r="G584" t="s">
-        <v>33</v>
+        <v>62</v>
       </c>
       <c r="H584" t="n">
         <v>2020</v>
@@ -31402,7 +31420,7 @@
         <v>2020</v>
       </c>
       <c r="G585" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="H585" t="n">
         <v>2020</v>
@@ -31452,7 +31470,7 @@
         <v>2020</v>
       </c>
       <c r="G586" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="H586" t="n">
         <v>2020</v>
@@ -31502,7 +31520,7 @@
         <v>2020</v>
       </c>
       <c r="G587" t="s">
-        <v>33</v>
+        <v>76</v>
       </c>
       <c r="H587" t="n">
         <v>2020</v>
@@ -31552,7 +31570,7 @@
         <v>2020</v>
       </c>
       <c r="G588" t="s">
-        <v>33</v>
+        <v>144</v>
       </c>
       <c r="H588" t="n">
         <v>2020</v>
@@ -31602,7 +31620,7 @@
         <v>2020</v>
       </c>
       <c r="G589" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="H589" t="n">
         <v>2020</v>
@@ -31652,7 +31670,7 @@
         <v>2020</v>
       </c>
       <c r="G590" t="s">
-        <v>33</v>
+        <v>150</v>
       </c>
       <c r="H590" t="n">
         <v>2020</v>
@@ -31702,7 +31720,7 @@
         <v>2020</v>
       </c>
       <c r="G591" t="s">
-        <v>33</v>
+        <v>154</v>
       </c>
       <c r="H591" t="n">
         <v>2020</v>
@@ -31752,7 +31770,7 @@
         <v>2020</v>
       </c>
       <c r="G592" t="s">
-        <v>33</v>
+        <v>52</v>
       </c>
       <c r="H592" t="n">
         <v>2020</v>
@@ -31802,7 +31820,7 @@
         <v>2020</v>
       </c>
       <c r="G593" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="H593" t="n">
         <v>2020</v>
@@ -31852,7 +31870,7 @@
         <v>2020</v>
       </c>
       <c r="G594" t="s">
-        <v>33</v>
+        <v>76</v>
       </c>
       <c r="H594" t="n">
         <v>2020</v>
@@ -31902,7 +31920,7 @@
         <v>2020</v>
       </c>
       <c r="G595" t="s">
-        <v>33</v>
+        <v>188</v>
       </c>
       <c r="H595" t="n">
         <v>2020</v>
@@ -31952,7 +31970,7 @@
         <v>2020</v>
       </c>
       <c r="G596" t="s">
-        <v>33</v>
+        <v>191</v>
       </c>
       <c r="H596" t="n">
         <v>2020</v>
@@ -32002,7 +32020,7 @@
         <v>2020</v>
       </c>
       <c r="G597" t="s">
-        <v>33</v>
+        <v>321</v>
       </c>
       <c r="H597" t="n">
         <v>2020</v>
@@ -32052,7 +32070,7 @@
         <v>2020</v>
       </c>
       <c r="G598" t="s">
-        <v>33</v>
+        <v>321</v>
       </c>
       <c r="H598" t="n">
         <v>2020</v>
@@ -32102,7 +32120,7 @@
         <v>2020</v>
       </c>
       <c r="G599" t="s">
-        <v>33</v>
+        <v>380</v>
       </c>
       <c r="H599" t="n">
         <v>2020</v>
@@ -32152,7 +32170,7 @@
         <v>2020</v>
       </c>
       <c r="G600" t="s">
-        <v>33</v>
+        <v>52</v>
       </c>
       <c r="H600" t="n">
         <v>2020</v>
@@ -32202,7 +32220,7 @@
         <v>2020</v>
       </c>
       <c r="G601" t="s">
-        <v>33</v>
+        <v>506</v>
       </c>
       <c r="H601" t="n">
         <v>2020</v>
@@ -32252,7 +32270,7 @@
         <v>2020</v>
       </c>
       <c r="G602" t="s">
-        <v>33</v>
+        <v>507</v>
       </c>
       <c r="H602" t="n">
         <v>2020</v>
@@ -32302,7 +32320,7 @@
         <v>2020</v>
       </c>
       <c r="G603" t="s">
-        <v>33</v>
+        <v>149</v>
       </c>
       <c r="H603" t="n">
         <v>2020</v>
@@ -44702,7 +44720,7 @@
         <v>2019</v>
       </c>
       <c r="G851" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="H851" t="n">
         <v>2019</v>
@@ -44752,7 +44770,7 @@
         <v>2019</v>
       </c>
       <c r="G852" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="H852" t="n">
         <v>2019</v>
@@ -44802,7 +44820,7 @@
         <v>2019</v>
       </c>
       <c r="G853" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="H853" t="n">
         <v>2019</v>
@@ -44852,7 +44870,7 @@
         <v>2019</v>
       </c>
       <c r="G854" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="H854" t="n">
         <v>2019</v>
@@ -44902,7 +44920,7 @@
         <v>2019</v>
       </c>
       <c r="G855" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="H855" t="n">
         <v>2019</v>
@@ -44952,7 +44970,7 @@
         <v>2019</v>
       </c>
       <c r="G856" t="s">
-        <v>33</v>
+        <v>52</v>
       </c>
       <c r="H856" t="n">
         <v>2019</v>
@@ -45002,7 +45020,7 @@
         <v>2019</v>
       </c>
       <c r="G857" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="H857" t="n">
         <v>2019</v>
@@ -45052,7 +45070,7 @@
         <v>2019</v>
       </c>
       <c r="G858" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="H858" t="n">
         <v>2019</v>
@@ -45102,7 +45120,7 @@
         <v>2019</v>
       </c>
       <c r="G859" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="H859" t="n">
         <v>2019</v>
@@ -45152,7 +45170,7 @@
         <v>2019</v>
       </c>
       <c r="G860" t="s">
-        <v>33</v>
+        <v>62</v>
       </c>
       <c r="H860" t="n">
         <v>2019</v>
@@ -45202,7 +45220,7 @@
         <v>2019</v>
       </c>
       <c r="G861" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="H861" t="n">
         <v>2019</v>
@@ -45252,7 +45270,7 @@
         <v>2019</v>
       </c>
       <c r="G862" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="H862" t="n">
         <v>2019</v>
@@ -45302,7 +45320,7 @@
         <v>2019</v>
       </c>
       <c r="G863" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="H863" t="n">
         <v>2019</v>
@@ -45352,7 +45370,7 @@
         <v>2019</v>
       </c>
       <c r="G864" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="H864" t="n">
         <v>2019</v>
@@ -45402,7 +45420,7 @@
         <v>2019</v>
       </c>
       <c r="G865" t="s">
-        <v>33</v>
+        <v>80</v>
       </c>
       <c r="H865" t="n">
         <v>2019</v>
@@ -45452,7 +45470,7 @@
         <v>2019</v>
       </c>
       <c r="G866" t="s">
-        <v>33</v>
+        <v>62</v>
       </c>
       <c r="H866" t="n">
         <v>2019</v>
@@ -45502,7 +45520,7 @@
         <v>2019</v>
       </c>
       <c r="G867" t="s">
-        <v>33</v>
+        <v>62</v>
       </c>
       <c r="H867" t="n">
         <v>2019</v>
@@ -45552,7 +45570,7 @@
         <v>2019</v>
       </c>
       <c r="G868" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="H868" t="n">
         <v>2019</v>
@@ -45602,7 +45620,7 @@
         <v>2019</v>
       </c>
       <c r="G869" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="H869" t="n">
         <v>2019</v>
@@ -45652,7 +45670,7 @@
         <v>2019</v>
       </c>
       <c r="G870" t="s">
-        <v>33</v>
+        <v>76</v>
       </c>
       <c r="H870" t="n">
         <v>2019</v>
@@ -45702,7 +45720,7 @@
         <v>2019</v>
       </c>
       <c r="G871" t="s">
-        <v>33</v>
+        <v>143</v>
       </c>
       <c r="H871" t="n">
         <v>2019</v>
@@ -45752,7 +45770,7 @@
         <v>2019</v>
       </c>
       <c r="G872" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="H872" t="n">
         <v>2019</v>
@@ -45802,7 +45820,7 @@
         <v>2019</v>
       </c>
       <c r="G873" t="s">
-        <v>33</v>
+        <v>149</v>
       </c>
       <c r="H873" t="n">
         <v>2019</v>
@@ -45852,7 +45870,7 @@
         <v>2019</v>
       </c>
       <c r="G874" t="s">
-        <v>33</v>
+        <v>154</v>
       </c>
       <c r="H874" t="n">
         <v>2019</v>
@@ -45902,7 +45920,7 @@
         <v>2019</v>
       </c>
       <c r="G875" t="s">
-        <v>33</v>
+        <v>52</v>
       </c>
       <c r="H875" t="n">
         <v>2019</v>
@@ -45952,7 +45970,7 @@
         <v>2019</v>
       </c>
       <c r="G876" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="H876" t="n">
         <v>2019</v>
@@ -46002,7 +46020,7 @@
         <v>2019</v>
       </c>
       <c r="G877" t="s">
-        <v>33</v>
+        <v>76</v>
       </c>
       <c r="H877" t="n">
         <v>2019</v>
@@ -46052,7 +46070,7 @@
         <v>2019</v>
       </c>
       <c r="G878" t="s">
-        <v>33</v>
+        <v>188</v>
       </c>
       <c r="H878" t="n">
         <v>2019</v>
@@ -46102,7 +46120,7 @@
         <v>2019</v>
       </c>
       <c r="G879" t="s">
-        <v>33</v>
+        <v>191</v>
       </c>
       <c r="H879" t="n">
         <v>2019</v>
@@ -46152,7 +46170,7 @@
         <v>2019</v>
       </c>
       <c r="G880" t="s">
-        <v>33</v>
+        <v>320</v>
       </c>
       <c r="H880" t="n">
         <v>2019</v>
@@ -46202,7 +46220,7 @@
         <v>2019</v>
       </c>
       <c r="G881" t="s">
-        <v>33</v>
+        <v>322</v>
       </c>
       <c r="H881" t="n">
         <v>2019</v>
@@ -46252,7 +46270,7 @@
         <v>2019</v>
       </c>
       <c r="G882" t="s">
-        <v>33</v>
+        <v>380</v>
       </c>
       <c r="H882" t="n">
         <v>2019</v>
@@ -46302,7 +46320,7 @@
         <v>2019</v>
       </c>
       <c r="G883" t="s">
-        <v>33</v>
+        <v>52</v>
       </c>
       <c r="H883" t="n">
         <v>2019</v>
@@ -46352,7 +46370,7 @@
         <v>2019</v>
       </c>
       <c r="G884" t="s">
-        <v>33</v>
+        <v>188</v>
       </c>
       <c r="H884" t="n">
         <v>2019</v>
@@ -46402,7 +46420,7 @@
         <v>2019</v>
       </c>
       <c r="G885" t="s">
-        <v>33</v>
+        <v>321</v>
       </c>
       <c r="H885" t="n">
         <v>2019</v>
@@ -46452,7 +46470,7 @@
         <v>2019</v>
       </c>
       <c r="G886" t="s">
-        <v>33</v>
+        <v>80</v>
       </c>
       <c r="H886" t="n">
         <v>2019</v>

</xml_diff>